<commit_message>
Detailed review of linear regression as well as need to solve for logistic regression (classification)
</commit_message>
<xml_diff>
--- a/6_ML_Combined_Courses/Notes/Lines_Excel_Linear Regression.xlsx
+++ b/6_ML_Combined_Courses/Notes/Lines_Excel_Linear Regression.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\4_Applied ML with Python\Practice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CourseraPlus\6_ML_Combined_Courses\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285A2DD1-A9B7-48A4-B4EF-68CF7039C334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" r:id="rId1"/>
-    <sheet name="Bill &amp; Tips" sheetId="3" r:id="rId2"/>
-    <sheet name="Reference" sheetId="2" r:id="rId3"/>
+    <sheet name="House_Price_Raw" sheetId="5" r:id="rId2"/>
+    <sheet name="House_Prices" sheetId="4" r:id="rId3"/>
+    <sheet name="Bill &amp; Tips" sheetId="3" r:id="rId4"/>
+    <sheet name="Reference" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="b">'Bill &amp; Tips'!$C$13</definedName>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Graph Values</t>
   </si>
@@ -157,17 +160,51 @@
   <si>
     <t>Deviations Squared</t>
   </si>
+  <si>
+    <t>House Prices Data</t>
+  </si>
+  <si>
+    <t>Sq. ft</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Fit Line</t>
+  </si>
+  <si>
+    <t>Area ^ 2</t>
+  </si>
+  <si>
+    <t>Area x Price</t>
+  </si>
+  <si>
+    <t>Approx. Line</t>
+  </si>
+  <si>
+    <t>y = w0 + w1 * x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w0 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w1 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value = </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="0.0000000"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -249,7 +286,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +308,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,9 +384,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -351,35 +394,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -395,25 +438,35 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="4" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -421,9 +474,9 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -441,7 +494,125 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -483,6 +654,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -650,7 +826,7 @@
             <c:numRef>
               <c:f>Simple!$C$4:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.5</c:v>
@@ -763,7 +939,7 @@
             <c:numRef>
               <c:f>Simple!$D$4:$D$10</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.9142857142857099</c:v>
@@ -992,7 +1168,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1086,7 +1262,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1094,6 +1269,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1149,6 +1325,1277 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>y-plot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> with generalized line</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>House_Price_Raw!$C$4:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>325000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>340000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>385000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>425000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>455000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9387-48AD-BB9D-A1A4995EDD14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trendline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>House_Price_Raw!$D$4:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>315050</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>341300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9387-48AD-BB9D-A1A4995EDD14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="95806880"/>
+        <c:axId val="95793152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="95806880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>X-Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95793152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95793152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="250000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Y-Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95806880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="0"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>y-plot</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> with generalized line</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>House_Prices!$C$4:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>325000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>340000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>385000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>425000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>455000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>510000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5109-4081-974E-BAAA59DE3656}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Trendline</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>House_Prices!$D$4:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>305992.66763685213</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>351407.14205753955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>378655.82670995186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>382288.98466360685</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>433153.19601477671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>462218.45964401658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>491283.72327325656</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5109-4081-974E-BAAA59DE3656}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="95806880"/>
+        <c:axId val="95793152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="95806880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>X-Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95793152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="95793152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="250000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Y-Values</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95806880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:pattFill prst="ltDnDiag">
+          <a:fgClr>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:fgClr>
+          <a:bgClr>
+            <a:schemeClr val="lt1"/>
+          </a:bgClr>
+        </a:pattFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
@@ -1172,7 +2619,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1235,7 +2681,7 @@
             <c:numRef>
               <c:f>'Bill &amp; Tips'!$D$5:$D$10</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
@@ -1293,7 +2739,7 @@
             <c:numRef>
               <c:f>'Bill &amp; Tips'!$I$5:$I$10</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00_-;\-* #,##0.00_-;_-* "-"??_-;_-@_-</c:formatCode>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>4.1512125534950073</c:v>
@@ -1432,7 +2878,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1555,7 +3000,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1584,7 +3028,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1665,7 +3109,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1673,6 +3116,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1784,6 +3228,80 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
   <cs:axisTitle>
@@ -2336,6 +3854,1108 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="232">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:alpha val="51000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2904,7 +5524,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99E59151-3BFE-46D4-B980-575D39354571}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2929,6 +5549,92 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>519111</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2672D4DE-3662-4475-8C9F-92736735EFFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>519111</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2917449F-62BB-4E83-8EAE-A61149D43BEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>223836</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -2945,7 +5651,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{535730AD-4C82-4CC5-8C12-E356F4591565}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2983,7 +5689,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADED61B2-CC9E-4257-9DF9-03C1D76A0C9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3041,7 +5747,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3084,7 +5796,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3104,7 +5816,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29D541DB-80B7-497F-844A-63A509B4252A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3134,8 +5846,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B3:F11" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="B3:F11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B3:F11" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="B3:F11" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3143,13 +5855,57 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="X" dataDxfId="3"/>
-    <tableColumn id="2" name="y" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="6" name="Plot" dataDxfId="1" dataCellStyle="Comma">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="X" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="y" dataDxfId="12" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Plot" dataDxfId="11" dataCellStyle="Comma">
       <calculatedColumnFormula>$F$15*Table1[[#This Row],[X]]+$C$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="X.y" dataDxfId="0"/>
-    <tableColumn id="4" name="X^2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="X.y" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="X^2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8BA4D2BA-162F-4ED9-BBF8-18C4C301077B}" name="Table134" displayName="Table134" ref="B3:F11" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="B3:F11" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{F575D6C8-7228-45EA-980D-D1FBCCEDF425}" name="Sq. ft" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{30BEF09C-4862-4E5D-923D-95494E6BF125}" name="Price" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{59F25E48-BE50-4602-A598-002156A1ECAD}" name="Approx. Line" dataDxfId="1" dataCellStyle="Comma">
+      <calculatedColumnFormula>$F$15*Table134[[#This Row],[Sq. ft]]+$C$15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{E75069A2-78E3-4649-A94A-6EB2E0B91CBE}" name="Area x Price" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{448807D9-6C6D-477B-B71E-A771C07B9150}" name="Area ^ 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09130089-70F2-4A1E-83DD-BB8BB40B88AE}" name="Table13" displayName="Table13" ref="B3:F11" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="B3:F11" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2F07BD4E-CC21-407D-A64D-0F85FEECCDCF}" name="Sq. ft" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{267AE8C7-C33B-43EA-B1EC-756C7F291096}" name="Price" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{B1B735DE-9754-4020-B351-96A2845807B3}" name="Fit Line" dataDxfId="6" dataCellStyle="Comma">
+      <calculatedColumnFormula>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{503DBADC-70AD-4622-8E60-40A7836F5CCB}" name="Area x Price" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8EC3BD8D-EFB2-4A56-A8E2-3E769AE0BF8E}" name="Area ^ 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3451,7 +6207,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3706,11 +6462,468 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7BF8BCB-177D-4ABD-BE45-FE28BEF36C95}">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1500</v>
+      </c>
+      <c r="C4" s="34">
+        <v>325000</v>
+      </c>
+      <c r="D4" s="14">
+        <f>$F$15*Table134[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>315050</v>
+      </c>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>1625</v>
+      </c>
+      <c r="C5" s="34">
+        <v>340000</v>
+      </c>
+      <c r="D5" s="14">
+        <f>$F$15*Table134[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>341300</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>1700</v>
+      </c>
+      <c r="C6" s="34">
+        <v>365000</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>1710</v>
+      </c>
+      <c r="C7" s="34">
+        <v>385000</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1850</v>
+      </c>
+      <c r="C8" s="34">
+        <v>425000</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>1930</v>
+      </c>
+      <c r="C9" s="34">
+        <v>455000</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>2010</v>
+      </c>
+      <c r="C10" s="34">
+        <v>510000</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="35">
+        <f t="shared" ref="B11:F11" si="0">SUM(B4:B10)</f>
+        <v>12325</v>
+      </c>
+      <c r="C11" s="35">
+        <f t="shared" si="0"/>
+        <v>2805000</v>
+      </c>
+      <c r="D11" s="35">
+        <f>$F$15*Table134[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>2588300</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="36">
+        <v>50</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="36">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="12" t="str">
+        <f>"y = "&amp;ROUNDUP(F15,4)&amp;" * x + ("&amp;ROUNDUP(C15,5)&amp;")"</f>
+        <v>y = 210 * x + (50)</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B529724-B510-48F2-BA16-DE87C992AFC7}">
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1500</v>
+      </c>
+      <c r="C4" s="34">
+        <v>325000</v>
+      </c>
+      <c r="D4" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>305992.66763685213</v>
+      </c>
+      <c r="E4" s="37">
+        <f>B4*C4</f>
+        <v>487500000</v>
+      </c>
+      <c r="F4" s="37">
+        <f t="shared" ref="F4:F10" si="0">B4*B4</f>
+        <v>2250000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>1625</v>
+      </c>
+      <c r="C5" s="34">
+        <v>340000</v>
+      </c>
+      <c r="D5" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>351407.14205753955</v>
+      </c>
+      <c r="E5" s="37">
+        <f t="shared" ref="E5:E10" si="1">B5*C5</f>
+        <v>552500000</v>
+      </c>
+      <c r="F5" s="37">
+        <f t="shared" si="0"/>
+        <v>2640625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>1700</v>
+      </c>
+      <c r="C6" s="34">
+        <v>365000</v>
+      </c>
+      <c r="D6" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>378655.82670995186</v>
+      </c>
+      <c r="E6" s="37">
+        <f t="shared" si="1"/>
+        <v>620500000</v>
+      </c>
+      <c r="F6" s="37">
+        <f t="shared" si="0"/>
+        <v>2890000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>1710</v>
+      </c>
+      <c r="C7" s="34">
+        <v>385000</v>
+      </c>
+      <c r="D7" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>382288.98466360685</v>
+      </c>
+      <c r="E7" s="37">
+        <f t="shared" si="1"/>
+        <v>658350000</v>
+      </c>
+      <c r="F7" s="37">
+        <f t="shared" si="0"/>
+        <v>2924100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>1850</v>
+      </c>
+      <c r="C8" s="34">
+        <v>425000</v>
+      </c>
+      <c r="D8" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>433153.19601477671</v>
+      </c>
+      <c r="E8" s="37">
+        <f t="shared" si="1"/>
+        <v>786250000</v>
+      </c>
+      <c r="F8" s="37">
+        <f t="shared" si="0"/>
+        <v>3422500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>1930</v>
+      </c>
+      <c r="C9" s="34">
+        <v>455000</v>
+      </c>
+      <c r="D9" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>462218.45964401658</v>
+      </c>
+      <c r="E9" s="37">
+        <f t="shared" si="1"/>
+        <v>878150000</v>
+      </c>
+      <c r="F9" s="37">
+        <f t="shared" si="0"/>
+        <v>3724900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>2010</v>
+      </c>
+      <c r="C10" s="34">
+        <v>510000</v>
+      </c>
+      <c r="D10" s="14">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>491283.72327325656</v>
+      </c>
+      <c r="E10" s="37">
+        <f t="shared" si="1"/>
+        <v>1025100000</v>
+      </c>
+      <c r="F10" s="37">
+        <f t="shared" si="0"/>
+        <v>4040100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="35">
+        <f t="shared" ref="B11:F11" si="2">SUM(B4:B10)</f>
+        <v>12325</v>
+      </c>
+      <c r="C11" s="35">
+        <f t="shared" si="2"/>
+        <v>2805000</v>
+      </c>
+      <c r="D11" s="35">
+        <f>$F$15*Table13[[#This Row],[Sq. ft]]+$C$15</f>
+        <v>4238886.1524683759</v>
+      </c>
+      <c r="E11" s="35">
+        <f t="shared" si="2"/>
+        <v>5008350000</v>
+      </c>
+      <c r="F11" s="35">
+        <f t="shared" si="2"/>
+        <v>21892225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="36">
+        <f>((C11*F11)-(B11*E11))/(7*F11-B11*B11)</f>
+        <v>-238981.02541139594</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="36">
+        <f>((7*E11)-(B11*C11))/(7*F11-B11^2)</f>
+        <v>363.31579536549873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12" t="str">
+        <f>"y = "&amp;ROUNDUP(F15,4)&amp;" * x + ("&amp;ROUNDUP(C15,5)&amp;")"</f>
+        <v>y = 363.3158 * x + (-238981.02542)</v>
+      </c>
+      <c r="F18" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4118,8 +7331,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>